<commit_message>
bulk part and active/deactive done
</commit_message>
<xml_diff>
--- a/public/Bulk-add-part-sample-sheet.xlsx
+++ b/public/Bulk-add-part-sample-sheet.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26502"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5F68EF41-DC27-4711-BBC6-B0D44D71AF50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{11B52848-1357-4E2B-A05B-29792B2BA6E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,9 +28,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Part-name</t>
+  </si>
+  <si>
+    <t>Part-color</t>
+  </si>
+  <si>
+    <t>Technical-qc</t>
   </si>
   <si>
     <t>Description</t>
@@ -40,13 +46,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF34314C"/>
+      <name val="Roboto"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -69,8 +81,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -385,24 +398,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12.140625" customWidth="1"/>
     <col min="2" max="2" width="12.5703125" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rdl-2 panel changes done ,repairt done page ,summery page ,and after rdl-2 close the tray wh person can receive and close,same like sp wh
</commit_message>
<xml_diff>
--- a/public/Bulk-add-part-sample-sheet.xlsx
+++ b/public/Bulk-add-part-sample-sheet.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26502"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26712"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{11B52848-1357-4E2B-A05B-29792B2BA6E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{526FFCF6-7B08-488F-AA81-CAF4ECE33DC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,9 +28,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Part-name</t>
+  </si>
+  <si>
+    <t>Sp-Category</t>
   </si>
   <si>
     <t>Part-color</t>
@@ -398,32 +401,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.140625" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" customWidth="1"/>
+    <col min="1" max="2" width="12.140625" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>